<commit_message>
menyesuaikan tampilan dashboard sesuai keinginan user
</commit_message>
<xml_diff>
--- a/cost & bbm 2022 sd 2025.xlsx
+++ b/cost & bbm 2022 sd 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Downloads\SPIL\bbm\Analisa BBM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343AA3BC-120B-497E-82DC-3C03E521B46E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929B22F7-5396-4B0C-848A-99961AD25968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{F88CA839-DB7F-4E60-9CFF-046C703DC5B0}"/>
   </bookViews>
@@ -1523,11 +1523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5915B8A4-606E-4D98-A929-6F2AE5EE112A}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:M249"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="F162" sqref="F162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1692,7 +1691,7 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1">
+    <row r="5" spans="1:13">
       <c r="A5" s="10">
         <v>3</v>
       </c>
@@ -1733,7 +1732,7 @@
         <v>8206</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1">
+    <row r="6" spans="1:13">
       <c r="A6" s="10">
         <v>4</v>
       </c>
@@ -1815,7 +1814,7 @@
         <v>2325</v>
       </c>
     </row>
-    <row r="8" spans="1:13" hidden="1">
+    <row r="8" spans="1:13">
       <c r="A8" s="10">
         <v>6</v>
       </c>
@@ -1856,7 +1855,7 @@
         <v>33100</v>
       </c>
     </row>
-    <row r="9" spans="1:13" hidden="1">
+    <row r="9" spans="1:13">
       <c r="A9" s="10">
         <v>7</v>
       </c>
@@ -1897,7 +1896,7 @@
         <v>13400</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1">
+    <row r="10" spans="1:13">
       <c r="A10" s="10">
         <v>8</v>
       </c>
@@ -1938,7 +1937,7 @@
         <v>7300</v>
       </c>
     </row>
-    <row r="11" spans="1:13" hidden="1">
+    <row r="11" spans="1:13">
       <c r="A11" s="10">
         <v>9</v>
       </c>
@@ -1979,7 +1978,7 @@
         <v>8350</v>
       </c>
     </row>
-    <row r="12" spans="1:13" hidden="1">
+    <row r="12" spans="1:13">
       <c r="A12" s="10">
         <v>10</v>
       </c>
@@ -2061,7 +2060,7 @@
         <v>2578</v>
       </c>
     </row>
-    <row r="14" spans="1:13" hidden="1">
+    <row r="14" spans="1:13">
       <c r="A14" s="10">
         <v>12</v>
       </c>
@@ -2102,7 +2101,7 @@
         <v>41237</v>
       </c>
     </row>
-    <row r="15" spans="1:13" hidden="1">
+    <row r="15" spans="1:13">
       <c r="A15" s="10">
         <v>13</v>
       </c>
@@ -2143,7 +2142,7 @@
         <v>16106</v>
       </c>
     </row>
-    <row r="16" spans="1:13" hidden="1">
+    <row r="16" spans="1:13">
       <c r="A16" s="10">
         <v>14</v>
       </c>
@@ -2184,7 +2183,7 @@
         <v>4915</v>
       </c>
     </row>
-    <row r="17" spans="1:13" hidden="1">
+    <row r="17" spans="1:13">
       <c r="A17" s="10">
         <v>15</v>
       </c>
@@ -2225,7 +2224,7 @@
         <v>3803</v>
       </c>
     </row>
-    <row r="18" spans="1:13" hidden="1">
+    <row r="18" spans="1:13">
       <c r="A18" s="10">
         <v>16</v>
       </c>
@@ -2266,7 +2265,7 @@
         <v>8623</v>
       </c>
     </row>
-    <row r="19" spans="1:13" hidden="1">
+    <row r="19" spans="1:13">
       <c r="A19" s="10">
         <v>17</v>
       </c>
@@ -2307,7 +2306,7 @@
         <v>65268</v>
       </c>
     </row>
-    <row r="20" spans="1:13" hidden="1">
+    <row r="20" spans="1:13">
       <c r="A20" s="10">
         <v>18</v>
       </c>
@@ -2348,7 +2347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" hidden="1">
+    <row r="21" spans="1:13">
       <c r="A21" s="10">
         <v>19</v>
       </c>
@@ -2717,7 +2716,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="30" spans="1:13" hidden="1">
+    <row r="30" spans="1:13">
       <c r="A30" s="10">
         <v>28</v>
       </c>
@@ -2758,7 +2757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" hidden="1">
+    <row r="31" spans="1:13">
       <c r="A31" s="10">
         <v>29</v>
       </c>
@@ -2799,7 +2798,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:13" hidden="1">
+    <row r="32" spans="1:13">
       <c r="A32" s="10">
         <v>30</v>
       </c>
@@ -2922,7 +2921,7 @@
         <v>14360</v>
       </c>
     </row>
-    <row r="35" spans="1:13" hidden="1">
+    <row r="35" spans="1:13">
       <c r="A35" s="10">
         <v>33</v>
       </c>
@@ -3209,7 +3208,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="42" spans="1:13" hidden="1">
+    <row r="42" spans="1:13">
       <c r="A42" s="10">
         <v>40</v>
       </c>
@@ -3250,7 +3249,7 @@
         <v>53056.23</v>
       </c>
     </row>
-    <row r="43" spans="1:13" hidden="1">
+    <row r="43" spans="1:13">
       <c r="A43" s="10">
         <v>41</v>
       </c>
@@ -3578,7 +3577,7 @@
         <v>4598.4799999999996</v>
       </c>
     </row>
-    <row r="51" spans="1:13" hidden="1">
+    <row r="51" spans="1:13">
       <c r="A51" s="10">
         <v>49</v>
       </c>
@@ -3619,7 +3618,7 @@
         <v>71353.86</v>
       </c>
     </row>
-    <row r="52" spans="1:13" hidden="1">
+    <row r="52" spans="1:13">
       <c r="A52" s="10">
         <v>50</v>
       </c>
@@ -3660,7 +3659,7 @@
         <v>75409.09</v>
       </c>
     </row>
-    <row r="53" spans="1:13" hidden="1">
+    <row r="53" spans="1:13">
       <c r="A53" s="10">
         <v>51</v>
       </c>
@@ -3701,7 +3700,7 @@
         <v>28014</v>
       </c>
     </row>
-    <row r="54" spans="1:13" hidden="1">
+    <row r="54" spans="1:13">
       <c r="A54" s="10">
         <v>52</v>
       </c>
@@ -3742,7 +3741,7 @@
         <v>65248.31</v>
       </c>
     </row>
-    <row r="55" spans="1:13" hidden="1">
+    <row r="55" spans="1:13">
       <c r="A55" s="10">
         <v>53</v>
       </c>
@@ -3783,7 +3782,7 @@
         <v>21269.75</v>
       </c>
     </row>
-    <row r="56" spans="1:13" hidden="1">
+    <row r="56" spans="1:13">
       <c r="A56" s="10">
         <v>54</v>
       </c>
@@ -3865,7 +3864,7 @@
         <v>1690</v>
       </c>
     </row>
-    <row r="58" spans="1:13" hidden="1">
+    <row r="58" spans="1:13">
       <c r="A58" s="10">
         <v>56</v>
       </c>
@@ -4070,7 +4069,7 @@
         <v>2000.25</v>
       </c>
     </row>
-    <row r="63" spans="1:13" hidden="1">
+    <row r="63" spans="1:13">
       <c r="A63" s="10">
         <v>61</v>
       </c>
@@ -4111,7 +4110,7 @@
         <v>48748.24</v>
       </c>
     </row>
-    <row r="64" spans="1:13" hidden="1">
+    <row r="64" spans="1:13">
       <c r="A64" s="10">
         <v>62</v>
       </c>
@@ -4152,7 +4151,7 @@
         <v>42290.71</v>
       </c>
     </row>
-    <row r="65" spans="1:13" hidden="1">
+    <row r="65" spans="1:13">
       <c r="A65" s="10">
         <v>63</v>
       </c>
@@ -4193,7 +4192,7 @@
         <v>9229.76</v>
       </c>
     </row>
-    <row r="66" spans="1:13" hidden="1">
+    <row r="66" spans="1:13">
       <c r="A66" s="10">
         <v>64</v>
       </c>
@@ -4234,7 +4233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:13" hidden="1">
+    <row r="67" spans="1:13">
       <c r="A67" s="10">
         <v>65</v>
       </c>
@@ -4275,7 +4274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:13" hidden="1">
+    <row r="68" spans="1:13">
       <c r="A68" s="10">
         <v>66</v>
       </c>
@@ -4316,7 +4315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:13" hidden="1">
+    <row r="69" spans="1:13">
       <c r="A69" s="10">
         <v>67</v>
       </c>
@@ -4357,7 +4356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:13" hidden="1">
+    <row r="70" spans="1:13">
       <c r="A70" s="10">
         <v>68</v>
       </c>
@@ -4398,7 +4397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:13" hidden="1">
+    <row r="71" spans="1:13">
       <c r="A71" s="10">
         <v>69</v>
       </c>
@@ -4439,7 +4438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:13" hidden="1">
+    <row r="72" spans="1:13">
       <c r="A72" s="10">
         <v>70</v>
       </c>
@@ -4480,7 +4479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:13" hidden="1">
+    <row r="73" spans="1:13">
       <c r="A73" s="10">
         <v>71</v>
       </c>
@@ -4521,7 +4520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:13" hidden="1">
+    <row r="74" spans="1:13">
       <c r="A74" s="10">
         <v>72</v>
       </c>
@@ -4562,7 +4561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:13" hidden="1">
+    <row r="75" spans="1:13">
       <c r="A75" s="10">
         <v>73</v>
       </c>
@@ -4603,7 +4602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:13" hidden="1">
+    <row r="76" spans="1:13">
       <c r="A76" s="10">
         <v>74</v>
       </c>
@@ -4644,7 +4643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:13" hidden="1">
+    <row r="77" spans="1:13">
       <c r="A77" s="10">
         <v>75</v>
       </c>
@@ -4685,7 +4684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:13" hidden="1">
+    <row r="78" spans="1:13">
       <c r="A78" s="10">
         <v>76</v>
       </c>
@@ -4726,7 +4725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:13" hidden="1">
+    <row r="79" spans="1:13">
       <c r="A79" s="10">
         <v>77</v>
       </c>
@@ -4767,7 +4766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:13" hidden="1">
+    <row r="80" spans="1:13">
       <c r="A80" s="10">
         <v>78</v>
       </c>
@@ -4808,7 +4807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:13" hidden="1">
+    <row r="81" spans="1:13">
       <c r="A81" s="10">
         <v>79</v>
       </c>
@@ -4849,7 +4848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:13" hidden="1">
+    <row r="82" spans="1:13">
       <c r="A82" s="10">
         <v>80</v>
       </c>
@@ -4890,7 +4889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:13" hidden="1">
+    <row r="83" spans="1:13">
       <c r="A83" s="10">
         <v>81</v>
       </c>
@@ -4931,7 +4930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:13" hidden="1">
+    <row r="84" spans="1:13">
       <c r="A84" s="10">
         <v>82</v>
       </c>
@@ -4972,7 +4971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:13" hidden="1">
+    <row r="85" spans="1:13">
       <c r="A85" s="10">
         <v>83</v>
       </c>
@@ -5013,7 +5012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:13" hidden="1">
+    <row r="86" spans="1:13">
       <c r="A86" s="10">
         <v>84</v>
       </c>
@@ -5054,7 +5053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:13" hidden="1">
+    <row r="87" spans="1:13">
       <c r="A87" s="10">
         <v>85</v>
       </c>
@@ -5095,7 +5094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:13" hidden="1">
+    <row r="88" spans="1:13">
       <c r="A88" s="10">
         <v>86</v>
       </c>
@@ -5136,7 +5135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:13" hidden="1">
+    <row r="89" spans="1:13">
       <c r="A89" s="10">
         <v>87</v>
       </c>
@@ -5177,7 +5176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:13" hidden="1">
+    <row r="90" spans="1:13">
       <c r="A90" s="10">
         <v>88</v>
       </c>
@@ -5218,7 +5217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:13" hidden="1">
+    <row r="91" spans="1:13">
       <c r="A91" s="10">
         <v>89</v>
       </c>
@@ -5259,7 +5258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:13" hidden="1">
+    <row r="92" spans="1:13">
       <c r="A92" s="10">
         <v>90</v>
       </c>
@@ -5300,7 +5299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:13" hidden="1">
+    <row r="93" spans="1:13">
       <c r="A93" s="10">
         <v>91</v>
       </c>
@@ -5341,7 +5340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:13" hidden="1">
+    <row r="94" spans="1:13">
       <c r="A94" s="10">
         <v>92</v>
       </c>
@@ -5382,7 +5381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:13" hidden="1">
+    <row r="95" spans="1:13">
       <c r="A95" s="10">
         <v>93</v>
       </c>
@@ -5423,7 +5422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:13" hidden="1">
+    <row r="96" spans="1:13">
       <c r="A96" s="10">
         <v>94</v>
       </c>
@@ -5464,7 +5463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:13" hidden="1">
+    <row r="97" spans="1:13">
       <c r="A97" s="10">
         <v>95</v>
       </c>
@@ -5505,7 +5504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:13" hidden="1">
+    <row r="98" spans="1:13">
       <c r="A98" s="10">
         <v>96</v>
       </c>
@@ -5546,7 +5545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:13" hidden="1">
+    <row r="99" spans="1:13">
       <c r="A99" s="10">
         <v>97</v>
       </c>
@@ -5587,7 +5586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:13" hidden="1">
+    <row r="100" spans="1:13">
       <c r="A100" s="10">
         <v>98</v>
       </c>
@@ -5628,7 +5627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:13" hidden="1">
+    <row r="101" spans="1:13">
       <c r="A101" s="10">
         <v>99</v>
       </c>
@@ -5669,7 +5668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:13" hidden="1">
+    <row r="102" spans="1:13">
       <c r="A102" s="10">
         <v>100</v>
       </c>
@@ -5710,7 +5709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:13" hidden="1">
+    <row r="103" spans="1:13">
       <c r="A103" s="10">
         <v>101</v>
       </c>
@@ -5751,7 +5750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:13" hidden="1">
+    <row r="104" spans="1:13">
       <c r="A104" s="10">
         <v>102</v>
       </c>
@@ -5792,7 +5791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:13" hidden="1">
+    <row r="105" spans="1:13">
       <c r="A105" s="10">
         <v>103</v>
       </c>
@@ -5874,7 +5873,7 @@
         <v>7800</v>
       </c>
     </row>
-    <row r="107" spans="1:13" hidden="1">
+    <row r="107" spans="1:13">
       <c r="A107" s="10">
         <v>105</v>
       </c>
@@ -6038,7 +6037,7 @@
         <v>1716.26</v>
       </c>
     </row>
-    <row r="111" spans="1:13" hidden="1">
+    <row r="111" spans="1:13">
       <c r="A111" s="10">
         <v>109</v>
       </c>
@@ -6284,7 +6283,7 @@
         <v>5983.96</v>
       </c>
     </row>
-    <row r="117" spans="1:13" hidden="1">
+    <row r="117" spans="1:13">
       <c r="A117" s="10">
         <v>115</v>
       </c>
@@ -6325,7 +6324,7 @@
         <v>53799.77</v>
       </c>
     </row>
-    <row r="118" spans="1:13" hidden="1">
+    <row r="118" spans="1:13">
       <c r="A118" s="10">
         <v>116</v>
       </c>
@@ -6366,7 +6365,7 @@
         <v>56153.5</v>
       </c>
     </row>
-    <row r="119" spans="1:13" hidden="1">
+    <row r="119" spans="1:13">
       <c r="A119" s="10">
         <v>117</v>
       </c>
@@ -6407,7 +6406,7 @@
         <v>40767.56</v>
       </c>
     </row>
-    <row r="120" spans="1:13" hidden="1">
+    <row r="120" spans="1:13">
       <c r="A120" s="10">
         <v>118</v>
       </c>
@@ -6858,7 +6857,7 @@
         <v>732.43</v>
       </c>
     </row>
-    <row r="131" spans="1:13" hidden="1">
+    <row r="131" spans="1:13">
       <c r="A131" s="10">
         <v>129</v>
       </c>
@@ -6899,7 +6898,7 @@
         <v>30968.76</v>
       </c>
     </row>
-    <row r="132" spans="1:13" hidden="1">
+    <row r="132" spans="1:13">
       <c r="A132" s="10">
         <v>130</v>
       </c>
@@ -6940,7 +6939,7 @@
         <v>55283.76</v>
       </c>
     </row>
-    <row r="133" spans="1:13" hidden="1">
+    <row r="133" spans="1:13">
       <c r="A133" s="10">
         <v>131</v>
       </c>
@@ -6981,7 +6980,7 @@
         <v>67487.13</v>
       </c>
     </row>
-    <row r="134" spans="1:13" hidden="1">
+    <row r="134" spans="1:13">
       <c r="A134" s="10">
         <v>132</v>
       </c>
@@ -7022,7 +7021,7 @@
         <v>22380.07</v>
       </c>
     </row>
-    <row r="135" spans="1:13" hidden="1">
+    <row r="135" spans="1:13">
       <c r="A135" s="10">
         <v>133</v>
       </c>
@@ -7063,7 +7062,7 @@
         <v>28029.360000000001</v>
       </c>
     </row>
-    <row r="136" spans="1:13" hidden="1">
+    <row r="136" spans="1:13">
       <c r="A136" s="10">
         <v>134</v>
       </c>
@@ -7104,7 +7103,7 @@
         <v>21698.07</v>
       </c>
     </row>
-    <row r="137" spans="1:13" hidden="1">
+    <row r="137" spans="1:13">
       <c r="A137" s="10">
         <v>135</v>
       </c>
@@ -7145,7 +7144,7 @@
         <v>29460.33</v>
       </c>
     </row>
-    <row r="138" spans="1:13" hidden="1">
+    <row r="138" spans="1:13">
       <c r="A138" s="10">
         <v>136</v>
       </c>
@@ -7186,7 +7185,7 @@
         <v>21116.29</v>
       </c>
     </row>
-    <row r="139" spans="1:13" hidden="1">
+    <row r="139" spans="1:13">
       <c r="A139" s="10">
         <v>137</v>
       </c>
@@ -7227,7 +7226,7 @@
         <v>23254.18</v>
       </c>
     </row>
-    <row r="140" spans="1:13" hidden="1">
+    <row r="140" spans="1:13">
       <c r="A140" s="10">
         <v>138</v>
       </c>
@@ -7268,7 +7267,7 @@
         <v>25220.51</v>
       </c>
     </row>
-    <row r="141" spans="1:13" hidden="1">
+    <row r="141" spans="1:13">
       <c r="A141" s="10">
         <v>139</v>
       </c>
@@ -7309,7 +7308,7 @@
         <v>24269.01</v>
       </c>
     </row>
-    <row r="142" spans="1:13" hidden="1">
+    <row r="142" spans="1:13">
       <c r="A142" s="10">
         <v>140</v>
       </c>
@@ -7350,7 +7349,7 @@
         <v>22840.07</v>
       </c>
     </row>
-    <row r="143" spans="1:13" hidden="1">
+    <row r="143" spans="1:13">
       <c r="A143" s="10">
         <v>141</v>
       </c>
@@ -7391,7 +7390,7 @@
         <v>27354.86</v>
       </c>
     </row>
-    <row r="144" spans="1:13" hidden="1">
+    <row r="144" spans="1:13">
       <c r="A144" s="10">
         <v>142</v>
       </c>
@@ -7432,7 +7431,7 @@
         <v>24348.5</v>
       </c>
     </row>
-    <row r="145" spans="1:13" hidden="1">
+    <row r="145" spans="1:13">
       <c r="A145" s="10">
         <v>143</v>
       </c>
@@ -7473,7 +7472,7 @@
         <v>21559.5</v>
       </c>
     </row>
-    <row r="146" spans="1:13" hidden="1">
+    <row r="146" spans="1:13">
       <c r="A146" s="10">
         <v>144</v>
       </c>
@@ -7514,7 +7513,7 @@
         <v>24883.66</v>
       </c>
     </row>
-    <row r="147" spans="1:13" hidden="1">
+    <row r="147" spans="1:13">
       <c r="A147" s="10">
         <v>145</v>
       </c>
@@ -7555,7 +7554,7 @@
         <v>23457.69</v>
       </c>
     </row>
-    <row r="148" spans="1:13" hidden="1">
+    <row r="148" spans="1:13">
       <c r="A148" s="10">
         <v>146</v>
       </c>
@@ -7596,7 +7595,7 @@
         <v>8679.1200000000008</v>
       </c>
     </row>
-    <row r="149" spans="1:13" hidden="1">
+    <row r="149" spans="1:13">
       <c r="A149" s="10">
         <v>147</v>
       </c>
@@ -7637,7 +7636,7 @@
         <v>26275.919999999998</v>
       </c>
     </row>
-    <row r="150" spans="1:13" hidden="1">
+    <row r="150" spans="1:13">
       <c r="A150" s="10">
         <v>148</v>
       </c>
@@ -7678,7 +7677,7 @@
         <v>19255.36</v>
       </c>
     </row>
-    <row r="151" spans="1:13" hidden="1">
+    <row r="151" spans="1:13">
       <c r="A151" s="10">
         <v>149</v>
       </c>
@@ -7719,7 +7718,7 @@
         <v>22348.15</v>
       </c>
     </row>
-    <row r="152" spans="1:13" hidden="1">
+    <row r="152" spans="1:13">
       <c r="A152" s="10">
         <v>150</v>
       </c>
@@ -7760,7 +7759,7 @@
         <v>15899.56</v>
       </c>
     </row>
-    <row r="153" spans="1:13" hidden="1">
+    <row r="153" spans="1:13">
       <c r="A153" s="10">
         <v>151</v>
       </c>
@@ -7883,7 +7882,7 @@
         <v>3460.54</v>
       </c>
     </row>
-    <row r="156" spans="1:13" hidden="1">
+    <row r="156" spans="1:13">
       <c r="A156" s="10">
         <v>154</v>
       </c>
@@ -7924,7 +7923,7 @@
         <v>35674.910000000003</v>
       </c>
     </row>
-    <row r="157" spans="1:13" hidden="1">
+    <row r="157" spans="1:13">
       <c r="A157" s="10">
         <v>155</v>
       </c>
@@ -7965,7 +7964,7 @@
         <v>62980.17</v>
       </c>
     </row>
-    <row r="158" spans="1:13" hidden="1">
+    <row r="158" spans="1:13">
       <c r="A158" s="10">
         <v>156</v>
       </c>
@@ -8006,7 +8005,7 @@
         <v>44232.32</v>
       </c>
     </row>
-    <row r="159" spans="1:13" hidden="1">
+    <row r="159" spans="1:13">
       <c r="A159" s="10">
         <v>157</v>
       </c>
@@ -8047,7 +8046,7 @@
         <v>17592.93</v>
       </c>
     </row>
-    <row r="160" spans="1:13" hidden="1">
+    <row r="160" spans="1:13">
       <c r="A160" s="10">
         <v>158</v>
       </c>
@@ -8088,7 +8087,7 @@
         <v>10413.35</v>
       </c>
     </row>
-    <row r="161" spans="1:13" hidden="1">
+    <row r="161" spans="1:13">
       <c r="A161" s="10">
         <v>159</v>
       </c>
@@ -8129,7 +8128,7 @@
         <v>15105.21</v>
       </c>
     </row>
-    <row r="162" spans="1:13" hidden="1">
+    <row r="162" spans="1:13">
       <c r="A162" s="10">
         <v>160</v>
       </c>
@@ -8170,7 +8169,7 @@
         <v>7373.44</v>
       </c>
     </row>
-    <row r="163" spans="1:13" hidden="1">
+    <row r="163" spans="1:13">
       <c r="A163" s="10">
         <v>161</v>
       </c>
@@ -8211,7 +8210,7 @@
         <v>13102.17</v>
       </c>
     </row>
-    <row r="164" spans="1:13" hidden="1">
+    <row r="164" spans="1:13">
       <c r="A164" s="10">
         <v>162</v>
       </c>
@@ -8252,7 +8251,7 @@
         <v>17867.61</v>
       </c>
     </row>
-    <row r="165" spans="1:13" hidden="1">
+    <row r="165" spans="1:13">
       <c r="A165" s="10">
         <v>163</v>
       </c>
@@ -8293,7 +8292,7 @@
         <v>20354.419999999998</v>
       </c>
     </row>
-    <row r="166" spans="1:13" hidden="1">
+    <row r="166" spans="1:13">
       <c r="A166" s="10">
         <v>164</v>
       </c>
@@ -8334,7 +8333,7 @@
         <v>21161.81</v>
       </c>
     </row>
-    <row r="167" spans="1:13" hidden="1">
+    <row r="167" spans="1:13">
       <c r="A167" s="10">
         <v>165</v>
       </c>
@@ -8375,7 +8374,7 @@
         <v>18764.73</v>
       </c>
     </row>
-    <row r="168" spans="1:13" hidden="1">
+    <row r="168" spans="1:13">
       <c r="A168" s="10">
         <v>166</v>
       </c>
@@ -8416,7 +8415,7 @@
         <v>21113.72</v>
       </c>
     </row>
-    <row r="169" spans="1:13" hidden="1">
+    <row r="169" spans="1:13">
       <c r="A169" s="10">
         <v>167</v>
       </c>
@@ -8457,7 +8456,7 @@
         <v>19394.189999999999</v>
       </c>
     </row>
-    <row r="170" spans="1:13" hidden="1">
+    <row r="170" spans="1:13">
       <c r="A170" s="10">
         <v>168</v>
       </c>
@@ -8498,7 +8497,7 @@
         <v>18676.830000000002</v>
       </c>
     </row>
-    <row r="171" spans="1:13" hidden="1">
+    <row r="171" spans="1:13">
       <c r="A171" s="10">
         <v>169</v>
       </c>
@@ -8539,7 +8538,7 @@
         <v>19190.900000000001</v>
       </c>
     </row>
-    <row r="172" spans="1:13" hidden="1">
+    <row r="172" spans="1:13">
       <c r="A172" s="10">
         <v>170</v>
       </c>
@@ -8580,7 +8579,7 @@
         <v>15926.21</v>
       </c>
     </row>
-    <row r="173" spans="1:13" hidden="1">
+    <row r="173" spans="1:13">
       <c r="A173" s="10">
         <v>171</v>
       </c>
@@ -8621,7 +8620,7 @@
         <v>18678.04</v>
       </c>
     </row>
-    <row r="174" spans="1:13" hidden="1">
+    <row r="174" spans="1:13">
       <c r="A174" s="10">
         <v>172</v>
       </c>
@@ -8662,7 +8661,7 @@
         <v>17269.560000000001</v>
       </c>
     </row>
-    <row r="175" spans="1:13" hidden="1">
+    <row r="175" spans="1:13">
       <c r="A175" s="10">
         <v>173</v>
       </c>
@@ -8703,7 +8702,7 @@
         <v>17762.47</v>
       </c>
     </row>
-    <row r="176" spans="1:13" hidden="1">
+    <row r="176" spans="1:13">
       <c r="A176" s="10">
         <v>174</v>
       </c>
@@ -8744,7 +8743,7 @@
         <v>18121.54</v>
       </c>
     </row>
-    <row r="177" spans="1:13" hidden="1">
+    <row r="177" spans="1:13">
       <c r="A177" s="10">
         <v>175</v>
       </c>
@@ -8785,7 +8784,7 @@
         <v>16727.669999999998</v>
       </c>
     </row>
-    <row r="178" spans="1:13" hidden="1">
+    <row r="178" spans="1:13">
       <c r="A178" s="10">
         <v>176</v>
       </c>
@@ -8826,7 +8825,7 @@
         <v>18228.23</v>
       </c>
     </row>
-    <row r="179" spans="1:13" hidden="1">
+    <row r="179" spans="1:13">
       <c r="A179" s="10">
         <v>177</v>
       </c>
@@ -8867,7 +8866,7 @@
         <v>20024.95</v>
       </c>
     </row>
-    <row r="180" spans="1:13" hidden="1">
+    <row r="180" spans="1:13">
       <c r="A180" s="10">
         <v>178</v>
       </c>
@@ -8908,7 +8907,7 @@
         <v>18821.18</v>
       </c>
     </row>
-    <row r="181" spans="1:13" hidden="1">
+    <row r="181" spans="1:13">
       <c r="A181" s="10">
         <v>179</v>
       </c>
@@ -8949,7 +8948,7 @@
         <v>21414.65</v>
       </c>
     </row>
-    <row r="182" spans="1:13" hidden="1">
+    <row r="182" spans="1:13">
       <c r="A182" s="10">
         <v>180</v>
       </c>
@@ -8990,7 +8989,7 @@
         <v>24479.919999999998</v>
       </c>
     </row>
-    <row r="183" spans="1:13" hidden="1">
+    <row r="183" spans="1:13">
       <c r="A183" s="10">
         <v>181</v>
       </c>
@@ -9031,7 +9030,7 @@
         <v>19083.060000000001</v>
       </c>
     </row>
-    <row r="184" spans="1:13" hidden="1">
+    <row r="184" spans="1:13">
       <c r="A184" s="10">
         <v>182</v>
       </c>
@@ -9072,7 +9071,7 @@
         <v>21616.62</v>
       </c>
     </row>
-    <row r="185" spans="1:13" hidden="1">
+    <row r="185" spans="1:13">
       <c r="A185" s="10">
         <v>183</v>
       </c>
@@ -9113,7 +9112,7 @@
         <v>19450.060000000001</v>
       </c>
     </row>
-    <row r="186" spans="1:13" hidden="1">
+    <row r="186" spans="1:13">
       <c r="A186" s="10">
         <v>184</v>
       </c>
@@ -9154,7 +9153,7 @@
         <v>14504.09</v>
       </c>
     </row>
-    <row r="187" spans="1:13" hidden="1">
+    <row r="187" spans="1:13">
       <c r="A187" s="10">
         <v>185</v>
       </c>
@@ -9195,7 +9194,7 @@
         <v>20565.27</v>
       </c>
     </row>
-    <row r="188" spans="1:13" hidden="1">
+    <row r="188" spans="1:13">
       <c r="A188" s="10">
         <v>186</v>
       </c>
@@ -9236,7 +9235,7 @@
         <v>20178.349999999999</v>
       </c>
     </row>
-    <row r="189" spans="1:13" hidden="1">
+    <row r="189" spans="1:13">
       <c r="A189" s="10">
         <v>187</v>
       </c>
@@ -9277,7 +9276,7 @@
         <v>22337.07</v>
       </c>
     </row>
-    <row r="190" spans="1:13" hidden="1">
+    <row r="190" spans="1:13">
       <c r="A190" s="10">
         <v>188</v>
       </c>
@@ -9318,7 +9317,7 @@
         <v>20642.689999999999</v>
       </c>
     </row>
-    <row r="191" spans="1:13" hidden="1">
+    <row r="191" spans="1:13">
       <c r="A191" s="10">
         <v>189</v>
       </c>
@@ -9359,7 +9358,7 @@
         <v>15677.34</v>
       </c>
     </row>
-    <row r="192" spans="1:13" hidden="1">
+    <row r="192" spans="1:13">
       <c r="A192" s="10">
         <v>190</v>
       </c>
@@ -9400,7 +9399,7 @@
         <v>18921.32</v>
       </c>
     </row>
-    <row r="193" spans="1:13" hidden="1">
+    <row r="193" spans="1:13">
       <c r="A193" s="10">
         <v>191</v>
       </c>
@@ -9441,7 +9440,7 @@
         <v>22517.31</v>
       </c>
     </row>
-    <row r="194" spans="1:13" hidden="1">
+    <row r="194" spans="1:13">
       <c r="A194" s="10">
         <v>192</v>
       </c>
@@ -9482,7 +9481,7 @@
         <v>18499.060000000001</v>
       </c>
     </row>
-    <row r="195" spans="1:13" hidden="1">
+    <row r="195" spans="1:13">
       <c r="A195" s="10">
         <v>193</v>
       </c>
@@ -9523,7 +9522,7 @@
         <v>49306.96</v>
       </c>
     </row>
-    <row r="196" spans="1:13" hidden="1">
+    <row r="196" spans="1:13">
       <c r="A196" s="10">
         <v>194</v>
       </c>
@@ -9564,7 +9563,7 @@
         <v>50897.760000000002</v>
       </c>
     </row>
-    <row r="197" spans="1:13" hidden="1">
+    <row r="197" spans="1:13">
       <c r="A197" s="10">
         <v>195</v>
       </c>
@@ -9605,7 +9604,7 @@
         <v>50580.44</v>
       </c>
     </row>
-    <row r="198" spans="1:13" hidden="1">
+    <row r="198" spans="1:13">
       <c r="A198" s="10">
         <v>196</v>
       </c>
@@ -9646,7 +9645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:13" hidden="1">
+    <row r="199" spans="1:13">
       <c r="A199" s="10">
         <v>197</v>
       </c>
@@ -9810,7 +9809,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="203" spans="1:13" hidden="1">
+    <row r="203" spans="1:13">
       <c r="A203" s="10">
         <v>201</v>
       </c>
@@ -9851,7 +9850,7 @@
         <v>26066</v>
       </c>
     </row>
-    <row r="204" spans="1:13" hidden="1">
+    <row r="204" spans="1:13">
       <c r="A204" s="10">
         <v>202</v>
       </c>
@@ -9892,7 +9891,7 @@
         <v>1925</v>
       </c>
     </row>
-    <row r="205" spans="1:13" hidden="1">
+    <row r="205" spans="1:13">
       <c r="A205" s="10">
         <v>203</v>
       </c>
@@ -9933,7 +9932,7 @@
         <v>3305</v>
       </c>
     </row>
-    <row r="206" spans="1:13" hidden="1">
+    <row r="206" spans="1:13">
       <c r="A206" s="10">
         <v>204</v>
       </c>
@@ -9974,7 +9973,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="207" spans="1:13" hidden="1">
+    <row r="207" spans="1:13">
       <c r="A207" s="10">
         <v>205</v>
       </c>
@@ -10015,7 +10014,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="208" spans="1:13" hidden="1">
+    <row r="208" spans="1:13">
       <c r="A208" s="10">
         <v>206</v>
       </c>
@@ -10138,7 +10137,7 @@
         <v>1622.27</v>
       </c>
     </row>
-    <row r="211" spans="1:13" hidden="1">
+    <row r="211" spans="1:13">
       <c r="A211" s="10">
         <v>209</v>
       </c>
@@ -10179,7 +10178,7 @@
         <v>7573</v>
       </c>
     </row>
-    <row r="212" spans="1:13" hidden="1">
+    <row r="212" spans="1:13">
       <c r="A212" s="10">
         <v>210</v>
       </c>
@@ -10220,7 +10219,7 @@
         <v>1698</v>
       </c>
     </row>
-    <row r="213" spans="1:13" hidden="1">
+    <row r="213" spans="1:13">
       <c r="A213" s="10">
         <v>211</v>
       </c>
@@ -10302,7 +10301,7 @@
         <v>3430</v>
       </c>
     </row>
-    <row r="215" spans="1:13" hidden="1">
+    <row r="215" spans="1:13">
       <c r="A215" s="10">
         <v>213</v>
       </c>
@@ -10343,7 +10342,7 @@
         <v>19530</v>
       </c>
     </row>
-    <row r="216" spans="1:13" hidden="1">
+    <row r="216" spans="1:13">
       <c r="A216" s="10">
         <v>214</v>
       </c>
@@ -10384,7 +10383,7 @@
         <v>1655</v>
       </c>
     </row>
-    <row r="217" spans="1:13" hidden="1">
+    <row r="217" spans="1:13">
       <c r="A217" s="10">
         <v>215</v>
       </c>
@@ -10466,7 +10465,7 @@
         <v>5457</v>
       </c>
     </row>
-    <row r="219" spans="1:13" hidden="1">
+    <row r="219" spans="1:13">
       <c r="A219" s="10">
         <v>217</v>
       </c>
@@ -10671,7 +10670,7 @@
         <v>4775</v>
       </c>
     </row>
-    <row r="224" spans="1:13" hidden="1">
+    <row r="224" spans="1:13">
       <c r="A224" s="10">
         <v>222</v>
       </c>
@@ -10712,7 +10711,7 @@
         <v>29805</v>
       </c>
     </row>
-    <row r="225" spans="1:13" hidden="1">
+    <row r="225" spans="1:13">
       <c r="A225" s="10">
         <v>223</v>
       </c>
@@ -10753,7 +10752,7 @@
         <v>22885</v>
       </c>
     </row>
-    <row r="226" spans="1:13" hidden="1">
+    <row r="226" spans="1:13">
       <c r="A226" s="10">
         <v>224</v>
       </c>
@@ -10794,7 +10793,7 @@
         <v>13890</v>
       </c>
     </row>
-    <row r="227" spans="1:13" hidden="1">
+    <row r="227" spans="1:13">
       <c r="A227" s="10">
         <v>225</v>
       </c>
@@ -10835,7 +10834,7 @@
         <v>11470</v>
       </c>
     </row>
-    <row r="228" spans="1:13" hidden="1">
+    <row r="228" spans="1:13">
       <c r="A228" s="10">
         <v>226</v>
       </c>
@@ -10917,7 +10916,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="230" spans="1:13" hidden="1">
+    <row r="230" spans="1:13">
       <c r="A230" s="10">
         <v>228</v>
       </c>
@@ -10999,7 +10998,7 @@
         <v>13265</v>
       </c>
     </row>
-    <row r="232" spans="1:13" hidden="1">
+    <row r="232" spans="1:13">
       <c r="A232" s="10">
         <v>230</v>
       </c>
@@ -11204,7 +11203,7 @@
         <v>1114.81</v>
       </c>
     </row>
-    <row r="237" spans="1:13" hidden="1">
+    <row r="237" spans="1:13">
       <c r="A237" s="10">
         <v>235</v>
       </c>
@@ -11245,7 +11244,7 @@
         <v>36469</v>
       </c>
     </row>
-    <row r="238" spans="1:13" hidden="1">
+    <row r="238" spans="1:13">
       <c r="A238" s="10">
         <v>236</v>
       </c>
@@ -11286,7 +11285,7 @@
         <v>29456</v>
       </c>
     </row>
-    <row r="239" spans="1:13" hidden="1">
+    <row r="239" spans="1:13">
       <c r="A239" s="10">
         <v>237</v>
       </c>
@@ -11327,7 +11326,7 @@
         <v>2192</v>
       </c>
     </row>
-    <row r="240" spans="1:13" hidden="1">
+    <row r="240" spans="1:13">
       <c r="A240" s="10">
         <v>238</v>
       </c>
@@ -11368,7 +11367,7 @@
         <v>5392</v>
       </c>
     </row>
-    <row r="241" spans="1:13" hidden="1">
+    <row r="241" spans="1:13">
       <c r="A241" s="10">
         <v>239</v>
       </c>
@@ -11409,7 +11408,7 @@
         <v>4087</v>
       </c>
     </row>
-    <row r="242" spans="1:13" hidden="1">
+    <row r="242" spans="1:13">
       <c r="A242" s="10">
         <v>240</v>
       </c>
@@ -11450,7 +11449,7 @@
         <v>4793</v>
       </c>
     </row>
-    <row r="243" spans="1:13" hidden="1">
+    <row r="243" spans="1:13">
       <c r="A243" s="10">
         <v>241</v>
       </c>
@@ -11491,7 +11490,7 @@
         <v>4546</v>
       </c>
     </row>
-    <row r="244" spans="1:13" hidden="1">
+    <row r="244" spans="1:13">
       <c r="A244" s="10">
         <v>242</v>
       </c>
@@ -11573,7 +11572,7 @@
         <v>7161</v>
       </c>
     </row>
-    <row r="246" spans="1:13" hidden="1">
+    <row r="246" spans="1:13">
       <c r="A246" s="10">
         <v>244</v>
       </c>
@@ -11614,7 +11613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:13" hidden="1">
+    <row r="247" spans="1:13">
       <c r="A247" s="10">
         <v>245</v>
       </c>
@@ -11655,7 +11654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:13" hidden="1">
+    <row r="248" spans="1:13">
       <c r="A248" s="10">
         <v>246</v>
       </c>
@@ -11696,7 +11695,7 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="249" spans="1:13" hidden="1">
+    <row r="249" spans="1:13">
       <c r="A249" s="10">
         <v>247</v>
       </c>
@@ -11739,11 +11738,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A2:M249" xr:uid="{5915B8A4-606E-4D98-A929-6F2AE5EE112A}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="FORKLIFT"/>
-      </filters>
-    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:M249">
       <sortCondition ref="A2:A249"/>
     </sortState>

</xml_diff>